<commit_message>
Desenvolvendo Texto em Testes
</commit_message>
<xml_diff>
--- a/Resultados modelos.xlsx
+++ b/Resultados modelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sp-xa\OneDrive\Área de Trabalho\Monografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F6B149-01FF-412D-83B6-1D813F2171A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89735D87-25A5-4818-BF33-01D2A7E2AD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3E7DF31-F0AA-47B6-B4E6-D5CD4DFCEB93}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3E7DF31-F0AA-47B6-B4E6-D5CD4DFCEB93}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="14">
   <si>
     <t>modelo</t>
-  </si>
-  <si>
-    <t>configuração</t>
   </si>
   <si>
     <t>Precision</t>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t>Tempo Treinamento</t>
-  </si>
-  <si>
-    <t>Tempo Teste</t>
   </si>
   <si>
     <t>Random Forest</t>
@@ -81,13 +75,16 @@
   <si>
     <t>Accuracy</t>
   </si>
+  <si>
+    <t>conf.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -154,7 +151,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -168,7 +165,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -179,6 +205,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E68F65C-2DF4-43DA-BC99-ECC83C20027C}" name="Tabela2" displayName="Tabela2" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:G1048576" xr:uid="{2E68F65C-2DF4-43DA-BC99-ECC83C20027C}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{DD0E67FD-4405-4D59-9A74-C506C07F181C}" name="modelo" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{ED158FFB-8476-418F-A658-13CDC1C98B96}" name="conf." dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9F771680-6C5E-48A1-9A10-9C376DEC44D5}" name="Precision" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{299971E0-E689-49E4-B52C-3152BB2281F2}" name="Recall" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B55D36EF-7946-4FBC-AB18-CB4A866F47CF}" name="F1" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{8C35A167-6C16-4A59-87DC-8EEF4680F98A}" name="Accuracy" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B9405F7D-17AB-48A0-90E3-6792DAC6D23D}" name="Tempo Treinamento" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,14 +522,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3FCDEB-9E24-40FA-99E7-9D2F18034D24}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="6" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -497,30 +544,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -544,7 +588,7 @@
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -568,7 +612,7 @@
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -592,7 +636,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -616,7 +660,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -640,7 +684,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -664,7 +708,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -688,7 +732,7 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="8">
         <v>2</v>
@@ -711,7 +755,7 @@
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="8">
         <v>2</v>
@@ -734,7 +778,7 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8">
         <v>2</v>
@@ -757,7 +801,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="8">
         <v>2</v>
@@ -780,7 +824,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="8">
         <v>2</v>
@@ -803,7 +847,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="8">
         <v>2</v>
@@ -826,7 +870,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="8">
         <v>2</v>
@@ -849,7 +893,7 @@
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" s="8">
         <v>3</v>
@@ -872,7 +916,7 @@
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" s="8">
         <v>3</v>
@@ -895,7 +939,7 @@
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="8">
         <v>3</v>
@@ -918,7 +962,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" s="8">
         <v>3</v>
@@ -941,7 +985,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="8">
         <v>3</v>
@@ -964,7 +1008,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="8">
         <v>3</v>
@@ -987,7 +1031,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="8">
         <v>3</v>
@@ -1010,7 +1054,7 @@
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23" s="8">
         <v>4</v>
@@ -1033,7 +1077,7 @@
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="8">
         <v>4</v>
@@ -1056,7 +1100,7 @@
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" s="8">
         <v>4</v>
@@ -1079,7 +1123,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="8">
         <v>4</v>
@@ -1102,7 +1146,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" s="8">
         <v>4</v>
@@ -1125,7 +1169,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="8">
         <v>4</v>
@@ -1148,7 +1192,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="8">
         <v>4</v>
@@ -1171,7 +1215,7 @@
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B30" s="8">
         <v>5</v>
@@ -1194,7 +1238,7 @@
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B31" s="8">
         <v>5</v>
@@ -1217,7 +1261,7 @@
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B32" s="8">
         <v>5</v>
@@ -1240,7 +1284,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" s="8">
         <v>5</v>
@@ -1263,7 +1307,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" s="8">
         <v>5</v>
@@ -1286,7 +1330,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" s="8">
         <v>5</v>
@@ -1309,7 +1353,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" s="8">
         <v>5</v>
@@ -1332,7 +1376,7 @@
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B37" s="8">
         <v>6</v>
@@ -1355,7 +1399,7 @@
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B38" s="8">
         <v>6</v>
@@ -1378,7 +1422,7 @@
     </row>
     <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="8">
         <v>6</v>
@@ -1401,7 +1445,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B40" s="8">
         <v>6</v>
@@ -1421,7 +1465,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" s="8">
         <v>6</v>
@@ -1441,7 +1485,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42" s="8">
         <v>6</v>
@@ -1464,7 +1508,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B43" s="8">
         <v>6</v>
@@ -1673,5 +1717,8 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>